<commit_message>
ip address change to 47.88.57.165 in sql file.
</commit_message>
<xml_diff>
--- a/project4413/src/main/resources/product_excel.xlsx
+++ b/project4413/src/main/resources/product_excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F57B33B-FF86-4899-A25C-2C9D1C11E511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1CE766-27DC-964E-9D14-AB2FC81987A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{0FA0F518-5FD8-6942-A8F7-3C844A52198C}"/>
+    <workbookView xWindow="8980" yWindow="29300" windowWidth="33600" windowHeight="20540" xr2:uid="{0FA0F518-5FD8-6942-A8F7-3C844A52198C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,19 +22,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
-    <t>http://59.110.172.187:8083/images/caomei2.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>新鲜的草莓</t>
   </si>
   <si>
-    <t>Fresh strawberries</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>品牌：进口大红草莓</t>
   </si>
   <si>
-    <t>Fresh strawberries 2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>新鲜的草莓2</t>
   </si>
   <si>
-    <t>Brand: imported large red strawberry</t>
+    <t>http://59.110.172.187:8083/images/caomei2.jpg</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -42,7 +39,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -408,24 +405,24 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="192" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="15.625" customWidth="1"/>
-    <col min="2" max="2" width="41.375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="41.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
       </c>
       <c r="D1">
         <v>18</v>
@@ -440,15 +437,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>18</v>

</xml_diff>